<commit_message>
chore: tried to enable skiping experience with 1/4 experience
</commit_message>
<xml_diff>
--- a/public/documents/Importuserselms.xlsx
+++ b/public/documents/Importuserselms.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\project\elms\frontend\frontend-service\public\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -100,6 +100,9 @@
   </si>
   <si>
     <t>RDF-123</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -397,9 +400,9 @@
   </sheetPr>
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O4" sqref="O4"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -413,7 +416,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -519,7 +522,9 @@
       <c r="AA2" s="6"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7">
+        <v>1</v>
+      </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>

</xml_diff>